<commit_message>
Address implicit any types in JSON sample
</commit_message>
<xml_diff>
--- a/docs/resources/samples/table-data-with-hyperlinks.xlsx
+++ b/docs/resources/samples/table-data-with-hyperlinks.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24320"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67A46FEB-3446-43E3-9573-88C145B0F0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\resources\samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EB8B8-6D42-41A2-8C79-3C698FF83896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlainTable" sheetId="2" r:id="rId1"/>
     <sheet name="WithHyperLink" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -117,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,14 +521,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -557,7 +562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -574,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -591,7 +596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -608,7 +613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -625,7 +630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -642,7 +647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -659,7 +664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -689,17 +694,17 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.73046875" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="6" max="6" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -739,7 +744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -759,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -779,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -799,7 +804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -819,7 +824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -839,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -859,7 +864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -881,17 +886,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Doc" xr:uid="{7D687237-A53F-40D5-8A0E-47324BE53D7F}"/>
-    <hyperlink ref="E3" r:id="rId2" display="Doc" xr:uid="{17C3F70F-432F-4283-9FE9-31B9689C3CC5}"/>
-    <hyperlink ref="E4" r:id="rId3" display="Doc" xr:uid="{50BAE14B-9F7C-4BE6-B598-23384DA39697}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7D687237-A53F-40D5-8A0E-47324BE53D7F}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{17C3F70F-432F-4283-9FE9-31B9689C3CC5}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{50BAE14B-9F7C-4BE6-B598-23384DA39697}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{B7187120-EDA5-4AEE-B695-7FB73F351023}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{68BF6167-BD98-4BD2-82C7-4C50864D96C8}"/>
     <hyperlink ref="E6" r:id="rId6" xr:uid="{97C631CA-2BBE-4E6A-B244-6D6EF1DAF2BB}"/>
     <hyperlink ref="E8:E9" r:id="rId7" display="Search " xr:uid="{0521B0B8-0B16-4C6E-B5DC-6A45C957DCFE}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{2DB6786A-BB8C-4438-9EB8-ADA731FE4C94}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{FC0ABE3C-0F42-4F61-B6AD-80A6EAD541BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[samples] (Export JSON) Address implicit any types in JSON sample (#377)
* Address implicit any types in JSON sample

* Update docs/resources/samples/get-table-data.md

Co-authored-by: Alison McKay <almckay@microsoft.com>

Co-authored-by: Alison McKay <almckay@microsoft.com>
</commit_message>
<xml_diff>
--- a/docs/resources/samples/table-data-with-hyperlinks.xlsx
+++ b/docs/resources/samples/table-data-with-hyperlinks.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23516"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24320"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67A46FEB-3446-43E3-9573-88C145B0F0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\resources\samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EB8B8-6D42-41A2-8C79-3C698FF83896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlainTable" sheetId="2" r:id="rId1"/>
     <sheet name="WithHyperLink" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -117,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,14 +521,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -557,7 +562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -574,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -591,7 +596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -608,7 +613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -625,7 +630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -642,7 +647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -659,7 +664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -689,17 +694,17 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.73046875" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="6" max="6" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -739,7 +744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -759,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -779,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -799,7 +804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -819,7 +824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -839,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -859,7 +864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -881,17 +886,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Doc" xr:uid="{7D687237-A53F-40D5-8A0E-47324BE53D7F}"/>
-    <hyperlink ref="E3" r:id="rId2" display="Doc" xr:uid="{17C3F70F-432F-4283-9FE9-31B9689C3CC5}"/>
-    <hyperlink ref="E4" r:id="rId3" display="Doc" xr:uid="{50BAE14B-9F7C-4BE6-B598-23384DA39697}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7D687237-A53F-40D5-8A0E-47324BE53D7F}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{17C3F70F-432F-4283-9FE9-31B9689C3CC5}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{50BAE14B-9F7C-4BE6-B598-23384DA39697}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{B7187120-EDA5-4AEE-B695-7FB73F351023}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{68BF6167-BD98-4BD2-82C7-4C50864D96C8}"/>
     <hyperlink ref="E6" r:id="rId6" xr:uid="{97C631CA-2BBE-4E6A-B244-6D6EF1DAF2BB}"/>
     <hyperlink ref="E8:E9" r:id="rId7" display="Search " xr:uid="{0521B0B8-0B16-4C6E-B5DC-6A45C957DCFE}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{2DB6786A-BB8C-4438-9EB8-ADA731FE4C94}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{FC0ABE3C-0F42-4F61-B6AD-80A6EAD541BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing corrupt hyperlink and changing headers
</commit_message>
<xml_diff>
--- a/docs/resources/samples/table-data-with-hyperlinks.xlsx
+++ b/docs/resources/samples/table-data-with-hyperlinks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24320"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25118"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\resources\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EB8B8-6D42-41A2-8C79-3C698FF83896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC0E3000-2642-45DA-A22C-A03CB35117ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlainTable" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -122,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,14 +522,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -562,7 +563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -579,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -596,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -613,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -630,7 +631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -647,7 +648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -664,7 +665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -694,17 +695,17 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.73046875" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="6" max="6" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -744,7 +745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -764,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -784,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -804,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -824,7 +825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -844,7 +845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -864,7 +865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -892,13 +893,12 @@
     <hyperlink ref="E5" r:id="rId4" xr:uid="{B7187120-EDA5-4AEE-B695-7FB73F351023}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{68BF6167-BD98-4BD2-82C7-4C50864D96C8}"/>
     <hyperlink ref="E6" r:id="rId6" xr:uid="{97C631CA-2BBE-4E6A-B244-6D6EF1DAF2BB}"/>
-    <hyperlink ref="E8:E9" r:id="rId7" display="Search " xr:uid="{0521B0B8-0B16-4C6E-B5DC-6A45C957DCFE}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{2DB6786A-BB8C-4438-9EB8-ADA731FE4C94}"/>
-    <hyperlink ref="E9" r:id="rId9" xr:uid="{FC0ABE3C-0F42-4F61-B6AD-80A6EAD541BB}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{FC0ABE3C-0F42-4F61-B6AD-80A6EAD541BB}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{4E8C6511-3536-4626-A441-AA09BF402114}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Excel] (Samples) Fixing corrupt hyperlink and changing headers in JSON data sample (#472)
* Fixing corrupt hyperlink and changing headers

* Update docs/resources/samples/get-table-data.md

Co-authored-by: Elizabeth Samuel <elizs@microsoft.com>

Co-authored-by: Elizabeth Samuel <elizs@microsoft.com>
</commit_message>
<xml_diff>
--- a/docs/resources/samples/table-data-with-hyperlinks.xlsx
+++ b/docs/resources/samples/table-data-with-hyperlinks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24320"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25118"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\resources\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EB8B8-6D42-41A2-8C79-3C698FF83896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC0E3000-2642-45DA-A22C-A03CB35117ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlainTable" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -122,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,14 +522,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -562,7 +563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -579,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -596,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -613,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -630,7 +631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -647,7 +648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -664,7 +665,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -694,17 +695,17 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.73046875" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" customWidth="1"/>
-    <col min="6" max="6" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -724,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -744,7 +745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -764,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -784,7 +785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -804,7 +805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -824,7 +825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -844,7 +845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -864,7 +865,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -892,13 +893,12 @@
     <hyperlink ref="E5" r:id="rId4" xr:uid="{B7187120-EDA5-4AEE-B695-7FB73F351023}"/>
     <hyperlink ref="E7" r:id="rId5" xr:uid="{68BF6167-BD98-4BD2-82C7-4C50864D96C8}"/>
     <hyperlink ref="E6" r:id="rId6" xr:uid="{97C631CA-2BBE-4E6A-B244-6D6EF1DAF2BB}"/>
-    <hyperlink ref="E8:E9" r:id="rId7" display="Search " xr:uid="{0521B0B8-0B16-4C6E-B5DC-6A45C957DCFE}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{2DB6786A-BB8C-4438-9EB8-ADA731FE4C94}"/>
-    <hyperlink ref="E9" r:id="rId9" xr:uid="{FC0ABE3C-0F42-4F61-B6AD-80A6EAD541BB}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{FC0ABE3C-0F42-4F61-B6AD-80A6EAD541BB}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{4E8C6511-3536-4626-A441-AA09BF402114}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>